<commit_message>
fix the dictionary and matching for race validation
</commit_message>
<xml_diff>
--- a/data/season/current_season/Season_Ladder.xlsx
+++ b/data/season/current_season/Season_Ladder.xlsx
@@ -534,111 +534,111 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Balance Triathlon Club</t>
+          <t>Newcastle Triathlon Club</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C5" t="n">
-        <v>238</v>
+        <v>319</v>
       </c>
       <c r="D5" t="n">
-        <v>328</v>
+        <v>394</v>
       </c>
       <c r="E5" t="n">
         <v>300</v>
       </c>
       <c r="F5" t="n">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Brighton Baths Athletic Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>90</v>
       </c>
       <c r="C6" t="n">
-        <v>174</v>
+        <v>238</v>
       </c>
       <c r="D6" t="n">
-        <v>264</v>
+        <v>328</v>
       </c>
       <c r="E6" t="n">
-        <v>264</v>
+        <v>300</v>
       </c>
       <c r="F6" t="n">
-        <v>36</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Newcastle Triathlon Club</t>
+          <t>Brighton Baths Athletic Club</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C7" t="n">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D7" t="n">
-        <v>213</v>
+        <v>264</v>
       </c>
       <c r="E7" t="n">
-        <v>150</v>
+        <v>264</v>
       </c>
       <c r="F7" t="n">
-        <v>138</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>STG Triathlon Club</t>
+          <t>Maitland Triathlon Club</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="C8" t="n">
-        <v>114</v>
+        <v>182</v>
       </c>
       <c r="D8" t="n">
-        <v>204</v>
+        <v>242</v>
       </c>
       <c r="E8" t="n">
-        <v>204</v>
+        <v>242</v>
       </c>
       <c r="F8" t="n">
-        <v>49</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Maitland Triathlon Club</t>
+          <t>STG Triathlon Club</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="C9" t="n">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="D9" t="n">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="E9" t="n">
-        <v>150</v>
+        <v>204</v>
       </c>
       <c r="F9" t="n">
-        <v>132</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10">
@@ -666,111 +666,111 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Singleton Triathlon Club</t>
+          <t>Tomaree Triathlon Club</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="C11" t="n">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="D11" t="n">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="E11" t="n">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="F11" t="n">
-        <v>24</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Forster Triathlon Club</t>
+          <t>Singleton Triathlon Club</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C12" t="n">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="D12" t="n">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E12" t="n">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F12" t="n">
-        <v>46</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Concord Triathlon Club</t>
+          <t>Central Coast Triathlon Club</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C13" t="n">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D13" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="E13" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="F13" t="n">
-        <v>59</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Pulse Performance</t>
+          <t>Concord Triathlon Club</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>60</v>
       </c>
       <c r="C14" t="n">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="D14" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="E14" t="n">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="F14" t="n">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Central Coast Triathlon Club</t>
+          <t>Pulse Performance</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C15" t="n">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D15" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="E15" t="n">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="F15" t="n">
-        <v>135</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
@@ -798,23 +798,23 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Tomaree Triathlon Club</t>
+          <t>Forster Triathlon Club</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C17" t="n">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="D17" t="n">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="E17" t="n">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F17" t="n">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test 2 new result files
</commit_message>
<xml_diff>
--- a/data/season/current_season/Season_Ladder.xlsx
+++ b/data/season/current_season/Season_Ladder.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,23 +468,23 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cronulla Triathlon Club</t>
+          <t>Balmoral Triathlon Club</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>596</v>
+        <v>73</v>
       </c>
       <c r="D2" t="n">
-        <v>686</v>
+        <v>88</v>
       </c>
       <c r="E2" t="n">
-        <v>300</v>
+        <v>88</v>
       </c>
       <c r="F2" t="n">
-        <v>217</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3">
@@ -494,327 +494,459 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>514</v>
+        <v>69</v>
       </c>
       <c r="D3" t="n">
-        <v>604</v>
+        <v>69</v>
       </c>
       <c r="E3" t="n">
-        <v>300</v>
+        <v>69</v>
       </c>
       <c r="F3" t="n">
-        <v>274</v>
+        <v>253</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Balmoral Triathlon Club</t>
+          <t>Panthers Triathlon Club</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="C4" t="n">
-        <v>494</v>
+        <v>42</v>
       </c>
       <c r="D4" t="n">
-        <v>584</v>
+        <v>57</v>
       </c>
       <c r="E4" t="n">
-        <v>300</v>
+        <v>57</v>
       </c>
       <c r="F4" t="n">
-        <v>174</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Newcastle Triathlon Club</t>
+          <t>Pulse Performance</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="C5" t="n">
-        <v>319</v>
+        <v>26</v>
       </c>
       <c r="D5" t="n">
-        <v>394</v>
+        <v>56</v>
       </c>
       <c r="E5" t="n">
-        <v>300</v>
+        <v>56</v>
       </c>
       <c r="F5" t="n">
-        <v>138</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Balance Triathlon Club</t>
+          <t>Moore Performance Triathlon Club</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="C6" t="n">
-        <v>238</v>
+        <v>25</v>
       </c>
       <c r="D6" t="n">
-        <v>328</v>
+        <v>55</v>
       </c>
       <c r="E6" t="n">
-        <v>300</v>
+        <v>55</v>
       </c>
       <c r="F6" t="n">
-        <v>140</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Brighton Baths Athletic Club</t>
+          <t>STG Triathlon Club</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="C7" t="n">
-        <v>174</v>
+        <v>35</v>
       </c>
       <c r="D7" t="n">
-        <v>264</v>
+        <v>50</v>
       </c>
       <c r="E7" t="n">
-        <v>264</v>
+        <v>50</v>
       </c>
       <c r="F7" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Maitland Triathlon Club</t>
+          <t>Cronulla Triathlon Club</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>182</v>
+        <v>46</v>
       </c>
       <c r="D8" t="n">
-        <v>242</v>
+        <v>46</v>
       </c>
       <c r="E8" t="n">
-        <v>242</v>
+        <v>46</v>
       </c>
       <c r="F8" t="n">
-        <v>132</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>STG Triathlon Club</t>
+          <t>Australian Chinese Dragon</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>90</v>
+        <v>30</v>
       </c>
       <c r="C9" t="n">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>204</v>
+        <v>30</v>
       </c>
       <c r="E9" t="n">
-        <v>204</v>
+        <v>30</v>
       </c>
       <c r="F9" t="n">
-        <v>49</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Manly Vipers Triathlon Club</t>
+          <t>Concord Triathlon Club</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="C10" t="n">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="D10" t="n">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="E10" t="n">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="F10" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tomaree Triathlon Club</t>
+          <t>Hunters Hills Triathlon Club</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C11" t="n">
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="D11" t="n">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="E11" t="n">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="F11" t="n">
-        <v>53</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Singleton Triathlon Club</t>
+          <t>Coogee Triathlon Club</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="D12" t="n">
-        <v>121</v>
+        <v>19</v>
       </c>
       <c r="E12" t="n">
-        <v>121</v>
+        <v>19</v>
       </c>
       <c r="F12" t="n">
-        <v>24</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Central Coast Triathlon Club</t>
+          <t>Macarthur Triathlon Club</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="D13" t="n">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="E13" t="n">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="F13" t="n">
-        <v>135</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Concord Triathlon Club</t>
+          <t>Engadine Triathlon Club</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="C14" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="E14" t="n">
-        <v>110</v>
+        <v>15</v>
       </c>
       <c r="F14" t="n">
-        <v>59</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Pulse Performance</t>
+          <t>Brighton Baths Athletic Club</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D15" t="n">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="E15" t="n">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="F15" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Macarthur Triathlon Club</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>53</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Forster Triathlon Club</t>
+          <t>BRAT Triathlon Club</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>46</v>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>FilOz Triathlon Club</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Hills Red Army</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Manly Vipers Triathlon Club</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Northern Suburbs Triathlon Club</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>South West Sydney Triathlon Club</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>TriMob</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="n">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
normalize club names in ICL data and run south coast r1 file
</commit_message>
<xml_diff>
--- a/data/season/current_season/Season_Ladder.xlsx
+++ b/data/season/current_season/Season_Ladder.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,440 +512,528 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Panthers Triathlon Club</t>
+          <t>Illawarra Triathlon Club</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>30</v>
       </c>
       <c r="C4" t="n">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D4" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="E4" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F4" t="n">
-        <v>135</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Moore Performance Triathlon Club</t>
+          <t>Panthers Triathlon Club</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C5" t="n">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="D5" t="n">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E5" t="n">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="F5" t="n">
-        <v>44</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>STG Triathlon Club</t>
+          <t>Moore Performance Triathlon Club</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>45</v>
       </c>
       <c r="C6" t="n">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="D6" t="n">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E6" t="n">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="F6" t="n">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Hills Triathlon Club</t>
+          <t>STG Triathlon Club</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C7" t="n">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D7" t="n">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E7" t="n">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F7" t="n">
-        <v>178</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Cronulla Triathlon Club</t>
+          <t>Kiama Triathlon Club</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C8" t="n">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D8" t="n">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E8" t="n">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="F8" t="n">
-        <v>207</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Balance Triathlon Club</t>
+          <t>Hills Triathlon Club</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>30</v>
       </c>
       <c r="C9" t="n">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D9" t="n">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="E9" t="n">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="F9" t="n">
-        <v>127</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Coogee Triathlon Club</t>
+          <t>Cronulla Triathlon Club</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C10" t="n">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="D10" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E10" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F10" t="n">
-        <v>119</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Pulse Performance</t>
+          <t>Balance Triathlon Club</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>30</v>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D11" t="n">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="E11" t="n">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="F11" t="n">
-        <v>31</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Engadine Triathlon Club</t>
+          <t>Eurocoast Triathlon Club</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>45</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D12" t="n">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="E12" t="n">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="F12" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Concord Triathlon Club</t>
+          <t>Coogee Triathlon Club</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>30</v>
       </c>
       <c r="C13" t="n">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D13" t="n">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="E13" t="n">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="F13" t="n">
-        <v>53</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BRAT Triathlon Club</t>
+          <t>Pulse Performance</t>
         </is>
       </c>
       <c r="B14" t="n">
         <v>30</v>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D14" t="n">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="E14" t="n">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F14" t="n">
-        <v>161</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Manly Vipers Triathlon Club</t>
+          <t>Concord Triathlon Club</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>30</v>
       </c>
       <c r="C15" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D15" t="n">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E15" t="n">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F15" t="n">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Macarthur Triathlon Club</t>
+          <t>Engadine Triathlon Club</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C16" t="n">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="E16" t="n">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="F16" t="n">
-        <v>69</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>FilOz Triathlon Club</t>
+          <t>Manly Vipers Triathlon Club</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>30</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D17" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E17" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F17" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Sydney South West Triathlon Club</t>
+          <t>BRAT Triathlon Club</t>
         </is>
       </c>
       <c r="B18" t="n">
         <v>30</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D18" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="E18" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F18" t="n">
-        <v>2</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Brighton Baths Athletic Club</t>
+          <t>Macarthur Triathlon Club</t>
         </is>
       </c>
       <c r="B19" t="n">
         <v>15</v>
       </c>
       <c r="C19" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D19" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E19" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F19" t="n">
-        <v>42</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Northern Suburbs Triathlon Club</t>
+          <t>Jervis Bay Triathlon Club</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>15</v>
       </c>
       <c r="C20" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D20" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="E20" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F20" t="n">
-        <v>67</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Australian Chinese Triathlon Club</t>
+          <t>FilOz Triathlon Club</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F21" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Hunters Hills Triathlon Club</t>
+          <t>Sydney South West Triathlon Club</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F22" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>Brighton Baths Athletic Club</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>15</v>
+      </c>
+      <c r="C23" t="n">
+        <v>9</v>
+      </c>
+      <c r="D23" t="n">
+        <v>24</v>
+      </c>
+      <c r="E23" t="n">
+        <v>24</v>
+      </c>
+      <c r="F23" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Northern Suburbs Triathlon Club</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>15</v>
+      </c>
+      <c r="C24" t="n">
+        <v>9</v>
+      </c>
+      <c r="D24" t="n">
+        <v>24</v>
+      </c>
+      <c r="E24" t="n">
+        <v>24</v>
+      </c>
+      <c r="F24" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Australian Chinese Triathlon Club</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Hunters Hills Triathlon Club</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>TriMob</t>
         </is>
       </c>
-      <c r="B23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="n">
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
         <v>43</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new output format test
</commit_message>
<xml_diff>
--- a/data/season/current_season/Season_Ladder.xlsx
+++ b/data/season/current_season/Season_Ladder.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,573 +468,155 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Warringah Triathlon Club</t>
+          <t>Tweed Valley Triathletes</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C2" t="n">
-        <v>109</v>
+        <v>24</v>
       </c>
       <c r="D2" t="n">
-        <v>139</v>
+        <v>69</v>
       </c>
       <c r="E2" t="n">
-        <v>139</v>
+        <v>69</v>
       </c>
       <c r="F2" t="n">
-        <v>253</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Balmoral Triathlon Club</t>
+          <t>Yamba Multisport</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C3" t="n">
-        <v>93</v>
+        <v>22</v>
       </c>
       <c r="D3" t="n">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="E3" t="n">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="F3" t="n">
-        <v>152</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Illawarra Triathlon Club</t>
+          <t>Byron Breakers</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C4" t="n">
-        <v>86</v>
+        <v>18</v>
       </c>
       <c r="D4" t="n">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="E4" t="n">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="F4" t="n">
-        <v>77</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Panthers Triathlon Club</t>
+          <t>Grafton Triathlon Club</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C5" t="n">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="D5" t="n">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="E5" t="n">
-        <v>109</v>
+        <v>62</v>
       </c>
       <c r="F5" t="n">
-        <v>135</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Moore Performance Triathlon Club</t>
+          <t>Ballina Triathlon Club</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>45</v>
       </c>
       <c r="C6" t="n">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="E6" t="n">
-        <v>99</v>
+        <v>59</v>
       </c>
       <c r="F6" t="n">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>STG Triathlon Club</t>
+          <t>Coffs Harbour Triathlon Club</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>45</v>
       </c>
       <c r="C7" t="n">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="D7" t="n">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="E7" t="n">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="F7" t="n">
-        <v>49</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Kiama Triathlon Club</t>
+          <t>Port Macquarie Triathlon Club</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C8" t="n">
-        <v>59</v>
+        <v>2</v>
       </c>
       <c r="D8" t="n">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="E8" t="n">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="F8" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Hills Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>30</v>
-      </c>
-      <c r="C9" t="n">
-        <v>54</v>
-      </c>
-      <c r="D9" t="n">
-        <v>84</v>
-      </c>
-      <c r="E9" t="n">
-        <v>84</v>
-      </c>
-      <c r="F9" t="n">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Cronulla Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>15</v>
-      </c>
-      <c r="C10" t="n">
-        <v>65</v>
-      </c>
-      <c r="D10" t="n">
-        <v>80</v>
-      </c>
-      <c r="E10" t="n">
-        <v>80</v>
-      </c>
-      <c r="F10" t="n">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Balance Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>30</v>
-      </c>
-      <c r="C11" t="n">
-        <v>43</v>
-      </c>
-      <c r="D11" t="n">
-        <v>73</v>
-      </c>
-      <c r="E11" t="n">
-        <v>73</v>
-      </c>
-      <c r="F11" t="n">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Eurocoast Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>45</v>
-      </c>
-      <c r="C12" t="n">
-        <v>26</v>
-      </c>
-      <c r="D12" t="n">
-        <v>71</v>
-      </c>
-      <c r="E12" t="n">
-        <v>71</v>
-      </c>
-      <c r="F12" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Coogee Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>30</v>
-      </c>
-      <c r="C13" t="n">
         <v>40</v>
-      </c>
-      <c r="D13" t="n">
-        <v>70</v>
-      </c>
-      <c r="E13" t="n">
-        <v>70</v>
-      </c>
-      <c r="F13" t="n">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Pulse Performance</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>30</v>
-      </c>
-      <c r="C14" t="n">
-        <v>26</v>
-      </c>
-      <c r="D14" t="n">
-        <v>56</v>
-      </c>
-      <c r="E14" t="n">
-        <v>56</v>
-      </c>
-      <c r="F14" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Concord Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>30</v>
-      </c>
-      <c r="C15" t="n">
-        <v>15</v>
-      </c>
-      <c r="D15" t="n">
-        <v>45</v>
-      </c>
-      <c r="E15" t="n">
-        <v>45</v>
-      </c>
-      <c r="F15" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Engadine Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>45</v>
-      </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>45</v>
-      </c>
-      <c r="E16" t="n">
-        <v>45</v>
-      </c>
-      <c r="F16" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Manly Vipers Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>30</v>
-      </c>
-      <c r="C17" t="n">
-        <v>9</v>
-      </c>
-      <c r="D17" t="n">
-        <v>39</v>
-      </c>
-      <c r="E17" t="n">
-        <v>39</v>
-      </c>
-      <c r="F17" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>BRAT Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>30</v>
-      </c>
-      <c r="C18" t="n">
-        <v>9</v>
-      </c>
-      <c r="D18" t="n">
-        <v>39</v>
-      </c>
-      <c r="E18" t="n">
-        <v>39</v>
-      </c>
-      <c r="F18" t="n">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Macarthur Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>15</v>
-      </c>
-      <c r="C19" t="n">
-        <v>19</v>
-      </c>
-      <c r="D19" t="n">
-        <v>34</v>
-      </c>
-      <c r="E19" t="n">
-        <v>34</v>
-      </c>
-      <c r="F19" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Jervis Bay Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>15</v>
-      </c>
-      <c r="C20" t="n">
-        <v>16</v>
-      </c>
-      <c r="D20" t="n">
-        <v>31</v>
-      </c>
-      <c r="E20" t="n">
-        <v>31</v>
-      </c>
-      <c r="F20" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>FilOz Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>30</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>30</v>
-      </c>
-      <c r="E21" t="n">
-        <v>30</v>
-      </c>
-      <c r="F21" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Sydney South West Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>30</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>30</v>
-      </c>
-      <c r="E22" t="n">
-        <v>30</v>
-      </c>
-      <c r="F22" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Brighton Baths Athletic Club</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>15</v>
-      </c>
-      <c r="C23" t="n">
-        <v>9</v>
-      </c>
-      <c r="D23" t="n">
-        <v>24</v>
-      </c>
-      <c r="E23" t="n">
-        <v>24</v>
-      </c>
-      <c r="F23" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Northern Suburbs Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>15</v>
-      </c>
-      <c r="C24" t="n">
-        <v>9</v>
-      </c>
-      <c r="D24" t="n">
-        <v>24</v>
-      </c>
-      <c r="E24" t="n">
-        <v>24</v>
-      </c>
-      <c r="F24" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Australian Chinese Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>0</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Hunters Hills Triathlon Club</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>TriMob</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>